<commit_message>
[TASK] Working on documentation
</commit_message>
<xml_diff>
--- a/documentation/20_time_evaluation/time_evaluation.xlsx
+++ b/documentation/20_time_evaluation/time_evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\case-study-2-database\documentation\20_time_evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Projekte\case-study-2-database\documentation\20_time_evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC060DC-EB5E-4946-8397-72E9721966AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF45A2B1-79A8-4B00-A1AE-84AF2B4EE0DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47730" yWindow="9630" windowWidth="7500" windowHeight="6000" xr2:uid="{09D3A5CE-FC1F-4249-821B-CAEA1FA401F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09D3A5CE-FC1F-4249-821B-CAEA1FA401F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Datum</t>
   </si>
@@ -49,10 +49,16 @@
     <t>MG</t>
   </si>
   <si>
-    <t>Aufsetzenprojekt auf Github</t>
-  </si>
-  <si>
     <t>Top Down View Diagram</t>
+  </si>
+  <si>
+    <t>Morphologische Analyse</t>
+  </si>
+  <si>
+    <t>Risk Managment</t>
+  </si>
+  <si>
+    <t>Aufsetzen Projekt auf Github</t>
   </si>
 </sst>
 </file>
@@ -418,18 +424,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CF3465-B739-4474-ACDB-8C1A12C57312}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43652</v>
       </c>
@@ -451,13 +457,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43653</v>
       </c>
@@ -465,10 +471,52 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43662</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43665</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43665</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -486,7 +534,7 @@
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[TASK] Add external files
</commit_message>
<xml_diff>
--- a/documentation/20_time_evaluation/time_evaluation.xlsx
+++ b/documentation/20_time_evaluation/time_evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Projekte\case-study-2-database\documentation\20_time_evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\case-study-2-database\documentation\20_time_evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF45A2B1-79A8-4B00-A1AE-84AF2B4EE0DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306421A7-DA3D-4699-A869-9E8E233AEEDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09D3A5CE-FC1F-4249-821B-CAEA1FA401F4}"/>
+    <workbookView xWindow="44100" yWindow="9630" windowWidth="7500" windowHeight="6000" xr2:uid="{09D3A5CE-FC1F-4249-821B-CAEA1FA401F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenerfassung" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -59,6 +59,33 @@
   </si>
   <si>
     <t>Aufsetzen Projekt auf Github</t>
+  </si>
+  <si>
+    <t>MVC Konzpt</t>
+  </si>
+  <si>
+    <t>Webpack aufsetzen</t>
+  </si>
+  <si>
+    <t>Dispatching</t>
+  </si>
+  <si>
+    <t>Umsetzung Datenbankanbindung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umsetzung Site and Date Managment </t>
+  </si>
+  <si>
+    <t>Umsetzung Comany und User Managment</t>
+  </si>
+  <si>
+    <t>Umsetzung Reservation Managment</t>
+  </si>
+  <si>
+    <t>ERM</t>
+  </si>
+  <si>
+    <t>Präsentation</t>
   </si>
 </sst>
 </file>
@@ -424,18 +451,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CF3465-B739-4474-ACDB-8C1A12C57312}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43652</v>
       </c>
@@ -463,7 +490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43653</v>
       </c>
@@ -477,7 +504,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43662</v>
       </c>
@@ -491,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43665</v>
       </c>
@@ -505,7 +532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43665</v>
       </c>
@@ -516,7 +543,139 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>2.5</v>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43686</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43689</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43693</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43714</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43715</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43721</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43723</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43732</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43734</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>SUM(D2:D15)</f>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -534,7 +693,7 @@
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>